<commit_message>
make a tag after change the data flow
</commit_message>
<xml_diff>
--- a/backend/src/test.xlsx
+++ b/backend/src/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\excel-parse\backend\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3BF094-53AF-4E89-8D21-C7C2126DA208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9625FD6-4E3E-42DE-8961-BFF0D852E1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33000" yWindow="8715" windowWidth="20955" windowHeight="10575" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34830" yWindow="5910" windowWidth="20955" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rootApp" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="681">
   <si>
     <t>Independent App</t>
   </si>
@@ -2065,17 +2065,13 @@
   </si>
   <si>
     <t>ToolsTalk2 SE</t>
-  </si>
-  <si>
-    <t>Sub Due Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2085,14 +2081,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -2122,7 +2110,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2464,11 +2452,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="A1:H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2512,8 +2504,8 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
-        <v>9</v>
+      <c r="G2" s="2">
+        <v>45556</v>
       </c>
       <c r="H2" t="s">
         <v>9</v>
@@ -3478,7 +3470,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:H40" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:H1 A3:H40 A2:F2 H2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -10076,10 +10068,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K55"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10087,13 +10079,13 @@
     <col min="1" max="1" width="31.58203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.08203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.08203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>609</v>
       </c>
@@ -10106,29 +10098,26 @@
       <c r="D1" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>681</v>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>613</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>613</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -10141,17 +10130,18 @@
       <c r="D2" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2">
+        <v>45494</v>
+      </c>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>615</v>
       </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -10164,17 +10154,18 @@
       <c r="D3" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2">
+        <v>45647</v>
+      </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>618</v>
       </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -10189,19 +10180,18 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -10216,19 +10206,18 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -10243,17 +10232,16 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -10268,19 +10256,18 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H7" s="1" t="s">
-        <v>14</v>
+        <v>623</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>623</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -10295,19 +10282,18 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -10322,19 +10308,18 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -10349,19 +10334,18 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -10376,19 +10360,18 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -10403,19 +10386,18 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -10429,16 +10411,15 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -10452,16 +10433,15 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -10475,16 +10455,15 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -10498,16 +10477,15 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -10521,16 +10499,15 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -10545,13 +10522,12 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -10566,19 +10542,18 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H19" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -10593,19 +10568,18 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -10620,19 +10594,18 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -10647,19 +10620,18 @@
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H22" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -10674,19 +10646,18 @@
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="G23" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H23" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -10701,19 +10672,18 @@
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -10728,19 +10698,18 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -10755,19 +10724,18 @@
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="H26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
@@ -10782,19 +10750,18 @@
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>644</v>
+      </c>
       <c r="H27" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="J27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
@@ -10809,19 +10776,18 @@
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>644</v>
+      </c>
       <c r="H28" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="J28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>36</v>
       </c>
@@ -10836,19 +10802,18 @@
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>648</v>
+      </c>
       <c r="H29" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="J29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -10863,19 +10828,18 @@
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="G30" s="1" t="s">
+        <v>648</v>
+      </c>
       <c r="H30" s="1" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
@@ -10890,19 +10854,18 @@
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="G31" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H31" s="1" t="s">
-        <v>14</v>
+        <v>645</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -10917,17 +10880,16 @@
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -10942,19 +10904,18 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="H33" s="1" t="s">
-        <v>37</v>
+        <v>645</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>645</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
@@ -10968,16 +10929,15 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>654</v>
+      </c>
       <c r="I34" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" s="1"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>48</v>
       </c>
@@ -10991,16 +10951,15 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>654</v>
+      </c>
       <c r="I35" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -11014,16 +10973,15 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="I36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K36" s="1"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -11037,16 +10995,15 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>654</v>
+      </c>
       <c r="I37" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -11060,16 +11017,15 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
+      <c r="H38" s="1" t="s">
+        <v>654</v>
+      </c>
       <c r="I38" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K38" s="1"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -11083,16 +11039,15 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>654</v>
+      </c>
       <c r="I39" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K39" s="1"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -11106,16 +11061,15 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
+      <c r="H40" s="1" t="s">
+        <v>654</v>
+      </c>
       <c r="I40" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K40" s="1"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>50</v>
       </c>
@@ -11130,19 +11084,18 @@
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>662</v>
+      </c>
       <c r="H41" s="1" t="s">
-        <v>662</v>
+        <v>52</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K41" s="1"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>55</v>
       </c>
@@ -11156,16 +11109,15 @@
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="I42" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
@@ -11179,16 +11131,15 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
+      <c r="H43" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="I43" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="J43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>55</v>
       </c>
@@ -11202,16 +11153,15 @@
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="I44" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="J44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>59</v>
       </c>
@@ -11226,13 +11176,12 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K45" s="1"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>67</v>
       </c>
@@ -11247,19 +11196,18 @@
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="G46" s="1" t="s">
+        <v>668</v>
+      </c>
       <c r="H46" s="1" t="s">
-        <v>668</v>
+        <v>69</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J46" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="K46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>67</v>
       </c>
@@ -11273,16 +11221,15 @@
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="I47" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>81</v>
       </c>
@@ -11297,17 +11244,16 @@
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K48" s="1"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+      <c r="I48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>87</v>
       </c>
@@ -11322,17 +11268,16 @@
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>672</v>
       </c>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K49" s="1"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
@@ -11347,17 +11292,16 @@
       </c>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K50" s="1"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H50" s="1"/>
+      <c r="I50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>91</v>
       </c>
@@ -11372,19 +11316,18 @@
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
+      <c r="G51" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="H51" s="1" t="s">
-        <v>92</v>
+        <v>675</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K51" s="1"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>97</v>
       </c>
@@ -11399,17 +11342,16 @@
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
+      <c r="G52" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I52" s="1" t="s">
         <v>98</v>
       </c>
+      <c r="I52" s="1"/>
       <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
@@ -11423,16 +11365,15 @@
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>678</v>
+      </c>
       <c r="I53" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K53" s="1"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>105</v>
       </c>
@@ -11447,19 +11388,18 @@
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
+      <c r="G54" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="H54" s="1" t="s">
-        <v>247</v>
+        <v>107</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J54" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K54" s="1"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>108</v>
       </c>
@@ -11474,17 +11414,16 @@
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
+      <c r="G55" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H55" s="1" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K55" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="J55" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>